<commit_message>
Update predict the end of the expiration.xlsx
UPDATE
</commit_message>
<xml_diff>
--- a/predict the end of the expiration.xlsx
+++ b/predict the end of the expiration.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\الأدوية منتهية الصلاحية وكيفية تجنب خساراتها المادية\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdel\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -240,13 +240,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -259,14 +252,36 @@
     <xf numFmtId="14" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -582,7 +597,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,374 +615,374 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="152.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="10" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="33" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="8">
+      <c r="A2" s="14">
         <v>100123</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="14">
         <v>10</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="14">
         <v>5</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="15">
         <f>C2/D2</f>
         <v>2</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="15">
         <f>E2*12</f>
         <v>24</v>
       </c>
-      <c r="G2" s="10">
+      <c r="G2" s="16">
         <v>44682</v>
       </c>
-      <c r="H2" s="10">
+      <c r="H2" s="16">
         <f ca="1">EDATE(NOW(),F2)</f>
-        <v>44402</v>
-      </c>
-      <c r="I2" s="19" t="str">
+        <v>44452</v>
+      </c>
+      <c r="I2" s="17" t="str">
         <f ca="1">IF(H2&gt;G2,"low Consumption rate will  cause to have a lot of expired"," good statues")</f>
         <v xml:space="preserve"> good statues</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="32.25" x14ac:dyDescent="0.5">
-      <c r="A3" s="11">
+      <c r="A3" s="18">
         <v>100124</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="18">
         <v>20</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="18">
         <v>10</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="19">
         <f t="shared" ref="E3:E11" si="0">C3/D3</f>
         <v>2</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="19">
         <f t="shared" ref="F3:F11" si="1">E3*12</f>
         <v>24</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="20">
         <v>44378</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="20">
         <f t="shared" ref="H3:H11" ca="1" si="2">EDATE(NOW(),F3)</f>
-        <v>44402</v>
-      </c>
-      <c r="I3" s="19" t="str">
+        <v>44452</v>
+      </c>
+      <c r="I3" s="17" t="str">
         <f t="shared" ref="I3:I12" ca="1" si="3">IF(H3&gt;G3,"low Consumption rate will  cause to have a lot of expired"," good statues")</f>
         <v>low Consumption rate will  cause to have a lot of expired</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="32.25" x14ac:dyDescent="0.5">
-      <c r="A4" s="8">
+      <c r="A4" s="14">
         <v>100125</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="14">
         <v>30</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="14">
         <v>30</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="15">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="15">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="16">
         <v>45870</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="16">
         <f t="shared" ca="1" si="2"/>
-        <v>44037</v>
-      </c>
-      <c r="I4" s="19" t="str">
+        <v>44087</v>
+      </c>
+      <c r="I4" s="17" t="str">
         <f t="shared" ca="1" si="3"/>
         <v xml:space="preserve"> good statues</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="32.25" x14ac:dyDescent="0.5">
-      <c r="A5" s="11">
+      <c r="A5" s="18">
         <v>100126</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="18">
         <v>40</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="18">
         <v>20</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="19">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="19">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="20">
         <v>45047</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="20">
         <f t="shared" ca="1" si="2"/>
-        <v>44402</v>
-      </c>
-      <c r="I5" s="19" t="str">
+        <v>44452</v>
+      </c>
+      <c r="I5" s="17" t="str">
         <f t="shared" ca="1" si="3"/>
         <v xml:space="preserve"> good statues</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="32.25" x14ac:dyDescent="0.5">
-      <c r="A6" s="8">
+      <c r="A6" s="14">
         <v>100127</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="14">
         <v>50</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="14">
         <v>10</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="15">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="15">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="16">
         <v>45292</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="16">
         <f t="shared" ca="1" si="2"/>
-        <v>45498</v>
-      </c>
-      <c r="I6" s="19" t="str">
+        <v>45548</v>
+      </c>
+      <c r="I6" s="17" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>low Consumption rate will  cause to have a lot of expired</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="32.25" x14ac:dyDescent="0.5">
-      <c r="A7" s="11">
+      <c r="A7" s="18">
         <v>100128</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="18">
         <v>60</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="18">
         <v>8</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="19">
         <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="19">
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="20">
         <v>44621</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="20">
         <f t="shared" ca="1" si="2"/>
-        <v>46412</v>
-      </c>
-      <c r="I7" s="19" t="str">
+        <v>46459</v>
+      </c>
+      <c r="I7" s="17" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>low Consumption rate will  cause to have a lot of expired</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="32.25" x14ac:dyDescent="0.5">
-      <c r="A8" s="8">
+      <c r="A8" s="14">
         <v>100129</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="14">
         <v>70</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="14">
         <v>70</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="15">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="15">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="16">
         <v>43586</v>
       </c>
-      <c r="H8" s="10">
+      <c r="H8" s="16">
         <f t="shared" ca="1" si="2"/>
-        <v>44037</v>
-      </c>
-      <c r="I8" s="19" t="str">
+        <v>44087</v>
+      </c>
+      <c r="I8" s="17" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>low Consumption rate will  cause to have a lot of expired</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="32.25" x14ac:dyDescent="0.5">
-      <c r="A9" s="11">
+      <c r="A9" s="18">
         <v>100130</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="18">
         <v>80</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="18">
         <v>60</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="19">
         <f t="shared" si="0"/>
         <v>1.3333333333333333</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="19">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="G9" s="13">
+      <c r="G9" s="20">
         <v>44105</v>
       </c>
-      <c r="H9" s="13">
+      <c r="H9" s="20">
         <f t="shared" ca="1" si="2"/>
-        <v>44160</v>
-      </c>
-      <c r="I9" s="19" t="str">
+        <v>44209</v>
+      </c>
+      <c r="I9" s="17" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>low Consumption rate will  cause to have a lot of expired</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="32.25" x14ac:dyDescent="0.5">
-      <c r="A10" s="8">
+      <c r="A10" s="14">
         <v>100131</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="14">
         <v>90</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="14">
         <v>10</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="15">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="15">
         <f t="shared" si="1"/>
         <v>108</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="16">
         <v>45870</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H10" s="16">
         <f t="shared" ca="1" si="2"/>
-        <v>46959</v>
-      </c>
-      <c r="I10" s="19" t="str">
+        <v>47009</v>
+      </c>
+      <c r="I10" s="17" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>low Consumption rate will  cause to have a lot of expired</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="32.25" x14ac:dyDescent="0.5">
-      <c r="A11" s="11">
+      <c r="A11" s="18">
         <v>100132</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="18">
         <v>100</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="18">
         <v>70</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="19">
         <f t="shared" si="0"/>
         <v>1.4285714285714286</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="19">
         <f t="shared" si="1"/>
         <v>17.142857142857142</v>
       </c>
-      <c r="G11" s="13">
+      <c r="G11" s="20">
         <v>45871</v>
       </c>
-      <c r="H11" s="13">
+      <c r="H11" s="20">
         <f t="shared" ca="1" si="2"/>
-        <v>44190</v>
-      </c>
-      <c r="I11" s="19" t="str">
+        <v>44240</v>
+      </c>
+      <c r="I11" s="17" t="str">
         <f t="shared" ca="1" si="3"/>
         <v xml:space="preserve"> good statues</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="32.25" x14ac:dyDescent="0.5">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="19" t="str">
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="17" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> good statues</v>
       </c>
@@ -984,23 +999,23 @@
       <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="21"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1094,10 +1109,12 @@
       <c r="H24" s="3"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="iOVfy0Z8Xzm5vaq9RrUHka791OcLPbCr6gxuEgDINiorYgW6hFNtv7lyP14wbHpjmOtIThB2zvOihCnJ5t+hwQ==" saltValue="d9ln9qcq6AGYXooRrp0vlA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A14:G15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>

</xml_diff>